<commit_message>
Files modified for setting up testing/reading initial test values. To be changed.
</commit_message>
<xml_diff>
--- a/InitialTestValues.xlsx
+++ b/InitialTestValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA - HungerStates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67441F16-63C2-4482-96EC-0FDDF1C448F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F28653-8AD4-4F41-9245-28B5466EBCC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10395" xr2:uid="{2755E7A2-B65B-4843-98C1-1521C9C3621F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>TestLength</t>
   </si>
@@ -437,7 +437,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="K2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>3000</v>
@@ -543,25 +543,151 @@
         <v>500</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="O2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B3">
+        <v>120</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>90</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>3000</v>
+      </c>
+      <c r="M3">
+        <v>500</v>
+      </c>
+      <c r="N3">
+        <v>0.4</v>
+      </c>
+      <c r="O3">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B4">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>90</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>3000</v>
+      </c>
+      <c r="M4">
+        <v>500</v>
+      </c>
+      <c r="N4">
+        <v>0.7</v>
+      </c>
+      <c r="O4">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B5">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>90</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>3000</v>
+      </c>
+      <c r="M5">
+        <v>500</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated test numbers for testing
</commit_message>
<xml_diff>
--- a/InitialTestValues.xlsx
+++ b/InitialTestValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA - HungerStates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F28653-8AD4-4F41-9245-28B5466EBCC0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02E0F67-1CA5-4D89-A63D-914AB322269F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10395" xr2:uid="{2755E7A2-B65B-4843-98C1-1521C9C3621F}"/>
   </bookViews>
@@ -72,16 +72,16 @@
     <t>MaxPlantMultiplyRate</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed map size column from data set and updated pre test initial values
</commit_message>
<xml_diff>
--- a/InitialTestValues.xlsx
+++ b/InitialTestValues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA - HungerStates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02E0F67-1CA5-4D89-A63D-914AB322269F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCC5BD0-A4A9-4FBD-AF23-B3EB68E5FA37}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10395" xr2:uid="{2755E7A2-B65B-4843-98C1-1521C9C3621F}"/>
   </bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,16 +507,16 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>120</v>
+        <v>301</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>30</v>
@@ -531,10 +531,10 @@
         <v>90</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L2">
         <v>3000</v>
@@ -554,7 +554,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>301</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -578,10 +578,10 @@
         <v>90</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L3">
         <v>3000</v>
@@ -601,7 +601,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>120</v>
+        <v>301</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -625,10 +625,10 @@
         <v>90</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L4">
         <v>3000</v>
@@ -648,7 +648,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>120</v>
+        <v>301</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -672,10 +672,10 @@
         <v>90</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L5">
         <v>3000</v>

</xml_diff>

<commit_message>
Added test numbers - still needs to be filled in
</commit_message>
<xml_diff>
--- a/InitialTestValues.xlsx
+++ b/InitialTestValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCC5BD0-A4A9-4FBD-AF23-B3EB68E5FA37}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABD249-B592-4519-A9CA-DBCC562110B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10395" xr2:uid="{2755E7A2-B65B-4843-98C1-1521C9C3621F}"/>
   </bookViews>
@@ -25,29 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>TestLength</t>
   </si>
   <si>
-    <t>OptimalRewardOn</t>
-  </si>
-  <si>
     <t>PreyPopulation</t>
   </si>
   <si>
     <t>PredatorPopulation</t>
   </si>
   <si>
-    <t>MinPlantMultiplyRate</t>
-  </si>
-  <si>
-    <t>MinPlantSpawnRate</t>
-  </si>
-  <si>
-    <t>MaxPlantSpawnRate</t>
-  </si>
-  <si>
     <t>HungerRate</t>
   </si>
   <si>
@@ -66,12 +54,6 @@
     <t>Tau</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>MaxPlantMultiplyRate</t>
-  </si>
-  <si>
     <t>000</t>
   </si>
   <si>
@@ -82,6 +64,318 @@
   </si>
   <si>
     <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>029</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>032</t>
+  </si>
+  <si>
+    <t>033</t>
+  </si>
+  <si>
+    <t>034</t>
+  </si>
+  <si>
+    <t>035</t>
+  </si>
+  <si>
+    <t>036</t>
+  </si>
+  <si>
+    <t>037</t>
+  </si>
+  <si>
+    <t>038</t>
+  </si>
+  <si>
+    <t>039</t>
+  </si>
+  <si>
+    <t>040</t>
+  </si>
+  <si>
+    <t>041</t>
+  </si>
+  <si>
+    <t>042</t>
+  </si>
+  <si>
+    <t>043</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
+    <t>045</t>
+  </si>
+  <si>
+    <t>046</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>048</t>
+  </si>
+  <si>
+    <t>049</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>051</t>
+  </si>
+  <si>
+    <t>052</t>
+  </si>
+  <si>
+    <t>053</t>
+  </si>
+  <si>
+    <t>054</t>
+  </si>
+  <si>
+    <t>055</t>
+  </si>
+  <si>
+    <t>056</t>
+  </si>
+  <si>
+    <t>057</t>
+  </si>
+  <si>
+    <t>058</t>
+  </si>
+  <si>
+    <t>059</t>
+  </si>
+  <si>
+    <t>060</t>
+  </si>
+  <si>
+    <t>061</t>
+  </si>
+  <si>
+    <t>062</t>
+  </si>
+  <si>
+    <t>063</t>
+  </si>
+  <si>
+    <t>064</t>
+  </si>
+  <si>
+    <t>065</t>
+  </si>
+  <si>
+    <t>066</t>
+  </si>
+  <si>
+    <t>067</t>
+  </si>
+  <si>
+    <t>068</t>
+  </si>
+  <si>
+    <t>069</t>
+  </si>
+  <si>
+    <t>070</t>
+  </si>
+  <si>
+    <t>071</t>
+  </si>
+  <si>
+    <t>072</t>
+  </si>
+  <si>
+    <t>073</t>
+  </si>
+  <si>
+    <t>074</t>
+  </si>
+  <si>
+    <t>075</t>
+  </si>
+  <si>
+    <t>076</t>
+  </si>
+  <si>
+    <t>077</t>
+  </si>
+  <si>
+    <t>078</t>
+  </si>
+  <si>
+    <t>079</t>
+  </si>
+  <si>
+    <t>080</t>
+  </si>
+  <si>
+    <t>081</t>
+  </si>
+  <si>
+    <t>082</t>
+  </si>
+  <si>
+    <t>083</t>
+  </si>
+  <si>
+    <t>084</t>
+  </si>
+  <si>
+    <t>085</t>
+  </si>
+  <si>
+    <t>086</t>
+  </si>
+  <si>
+    <t>087</t>
+  </si>
+  <si>
+    <t>088</t>
+  </si>
+  <si>
+    <t>089</t>
+  </si>
+  <si>
+    <t>090</t>
+  </si>
+  <si>
+    <t>091</t>
+  </si>
+  <si>
+    <t>092</t>
+  </si>
+  <si>
+    <t>093</t>
+  </si>
+  <si>
+    <t>094</t>
+  </si>
+  <si>
+    <t>095</t>
+  </si>
+  <si>
+    <t>096</t>
+  </si>
+  <si>
+    <t>097</t>
+  </si>
+  <si>
+    <t>098</t>
+  </si>
+  <si>
+    <t>099</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
   </si>
 </sst>
 </file>
@@ -434,31 +728,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D409FE-4167-4C13-914B-04CE0AA514C1}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -475,89 +764,59 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="B2">
         <v>301</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="H2">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="I2">
-        <v>90</v>
+        <v>0.1</v>
       </c>
       <c r="J2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>301</v>
+      </c>
+      <c r="C3">
         <v>5</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>3000</v>
-      </c>
-      <c r="M2">
-        <v>500</v>
-      </c>
-      <c r="N2">
-        <v>0.1</v>
-      </c>
-      <c r="O2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <v>301</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -566,45 +825,30 @@
         <v>5</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="H3">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="I3">
-        <v>90</v>
+        <v>0.4</v>
       </c>
       <c r="J3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>301</v>
+      </c>
+      <c r="C4">
         <v>5</v>
-      </c>
-      <c r="K3">
-        <v>10</v>
-      </c>
-      <c r="L3">
-        <v>3000</v>
-      </c>
-      <c r="M3">
-        <v>500</v>
-      </c>
-      <c r="N3">
-        <v>0.4</v>
-      </c>
-      <c r="O3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>301</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -613,45 +857,30 @@
         <v>5</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G4">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="H4">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="I4">
-        <v>90</v>
+        <v>0.7</v>
       </c>
       <c r="J4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>301</v>
+      </c>
+      <c r="C5">
         <v>5</v>
-      </c>
-      <c r="K4">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>3000</v>
-      </c>
-      <c r="M4">
-        <v>500</v>
-      </c>
-      <c r="N4">
-        <v>0.7</v>
-      </c>
-      <c r="O4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <v>301</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -660,35 +889,855 @@
         <v>5</v>
       </c>
       <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>3000</v>
+      </c>
+      <c r="H5">
+        <v>500</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5">
+      <c r="B23">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H5">
-        <v>60</v>
-      </c>
-      <c r="I5">
+      <c r="B53">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J5">
-        <v>5</v>
-      </c>
-      <c r="K5">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <v>3000</v>
-      </c>
-      <c r="M5">
-        <v>500</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
+      <c r="B83">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B89">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B90">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B91">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B94">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B95">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B96">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B97">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B98">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B100">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B101">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B102">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B104">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B105">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B106">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B108">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B109">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed OptimalRewardOn and Plant Rates as no longer necessary. Updated initial values for all tests (up to 080)
</commit_message>
<xml_diff>
--- a/InitialTestValues.xlsx
+++ b/InitialTestValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABD249-B592-4519-A9CA-DBCC562110B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29BE736-90E4-4783-8EF5-4E332BC190B5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10395" xr2:uid="{2755E7A2-B65B-4843-98C1-1521C9C3621F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="93">
   <si>
     <t>TestLength</t>
   </si>
@@ -297,85 +297,13 @@
     <t>080</t>
   </si>
   <si>
-    <t>081</t>
-  </si>
-  <si>
-    <t>082</t>
-  </si>
-  <si>
-    <t>083</t>
-  </si>
-  <si>
-    <t>084</t>
-  </si>
-  <si>
-    <t>085</t>
-  </si>
-  <si>
-    <t>086</t>
-  </si>
-  <si>
-    <t>087</t>
-  </si>
-  <si>
-    <t>088</t>
-  </si>
-  <si>
-    <t>089</t>
-  </si>
-  <si>
-    <t>090</t>
-  </si>
-  <si>
-    <t>091</t>
-  </si>
-  <si>
-    <t>092</t>
-  </si>
-  <si>
-    <t>093</t>
-  </si>
-  <si>
-    <t>094</t>
-  </si>
-  <si>
-    <t>095</t>
-  </si>
-  <si>
-    <t>096</t>
-  </si>
-  <si>
-    <t>097</t>
-  </si>
-  <si>
-    <t>098</t>
-  </si>
-  <si>
-    <t>099</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>107</t>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>HIGH</t>
   </si>
 </sst>
 </file>
@@ -728,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D409FE-4167-4C13-914B-04CE0AA514C1}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,26 +711,26 @@
       <c r="B2">
         <v>301</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="H2">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="I2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="J2">
         <v>0.1</v>
@@ -815,29 +743,29 @@
       <c r="B3">
         <v>301</v>
       </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="H3">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="I3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="J3">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -847,29 +775,29 @@
       <c r="B4">
         <v>301</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="H4">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="I4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="J4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -879,29 +807,29 @@
       <c r="B5">
         <v>301</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="H5">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -911,6 +839,30 @@
       <c r="B6">
         <v>301</v>
       </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>3500</v>
+      </c>
+      <c r="H6">
+        <v>600</v>
+      </c>
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+      <c r="J6">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -919,6 +871,30 @@
       <c r="B7">
         <v>301</v>
       </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>3500</v>
+      </c>
+      <c r="H7">
+        <v>600</v>
+      </c>
+      <c r="I7">
+        <v>0.5</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -927,6 +903,30 @@
       <c r="B8">
         <v>301</v>
       </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>3500</v>
+      </c>
+      <c r="H8">
+        <v>600</v>
+      </c>
+      <c r="I8">
+        <v>0.8</v>
+      </c>
+      <c r="J8">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -935,6 +935,30 @@
       <c r="B9">
         <v>301</v>
       </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>3500</v>
+      </c>
+      <c r="H9">
+        <v>600</v>
+      </c>
+      <c r="I9">
+        <v>0.8</v>
+      </c>
+      <c r="J9">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -943,6 +967,30 @@
       <c r="B10">
         <v>301</v>
       </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>3500</v>
+      </c>
+      <c r="H10">
+        <v>600</v>
+      </c>
+      <c r="I10">
+        <v>0.8</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -951,6 +999,30 @@
       <c r="B11">
         <v>301</v>
       </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
+        <v>3500</v>
+      </c>
+      <c r="H11">
+        <v>600</v>
+      </c>
+      <c r="I11">
+        <v>0.2</v>
+      </c>
+      <c r="J11">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -959,6 +1031,30 @@
       <c r="B12">
         <v>301</v>
       </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>3500</v>
+      </c>
+      <c r="H12">
+        <v>600</v>
+      </c>
+      <c r="I12">
+        <v>0.2</v>
+      </c>
+      <c r="J12">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -967,6 +1063,30 @@
       <c r="B13">
         <v>301</v>
       </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>3500</v>
+      </c>
+      <c r="H13">
+        <v>600</v>
+      </c>
+      <c r="I13">
+        <v>0.2</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -975,6 +1095,30 @@
       <c r="B14">
         <v>301</v>
       </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>3500</v>
+      </c>
+      <c r="H14">
+        <v>600</v>
+      </c>
+      <c r="I14">
+        <v>0.5</v>
+      </c>
+      <c r="J14">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -983,6 +1127,30 @@
       <c r="B15">
         <v>301</v>
       </c>
+      <c r="C15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>3500</v>
+      </c>
+      <c r="H15">
+        <v>600</v>
+      </c>
+      <c r="I15">
+        <v>0.5</v>
+      </c>
+      <c r="J15">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -991,755 +1159,2148 @@
       <c r="B16">
         <v>301</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>3500</v>
+      </c>
+      <c r="H16">
+        <v>600</v>
+      </c>
+      <c r="I16">
+        <v>0.5</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B17">
         <v>301</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17">
+        <v>3500</v>
+      </c>
+      <c r="H17">
+        <v>600</v>
+      </c>
+      <c r="I17">
+        <v>0.8</v>
+      </c>
+      <c r="J17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B18">
         <v>301</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>3500</v>
+      </c>
+      <c r="H18">
+        <v>600</v>
+      </c>
+      <c r="I18">
+        <v>0.8</v>
+      </c>
+      <c r="J18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B19">
         <v>301</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>3500</v>
+      </c>
+      <c r="H19">
+        <v>600</v>
+      </c>
+      <c r="I19">
+        <v>0.8</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B20">
         <v>301</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>3500</v>
+      </c>
+      <c r="H20">
+        <v>600</v>
+      </c>
+      <c r="I20">
+        <v>0.2</v>
+      </c>
+      <c r="J20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B21">
         <v>301</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>3500</v>
+      </c>
+      <c r="H21">
+        <v>600</v>
+      </c>
+      <c r="I21">
+        <v>0.2</v>
+      </c>
+      <c r="J21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B22">
         <v>301</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>3500</v>
+      </c>
+      <c r="H22">
+        <v>600</v>
+      </c>
+      <c r="I22">
+        <v>0.2</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B23">
         <v>301</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23">
+        <v>10</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>3500</v>
+      </c>
+      <c r="H23">
+        <v>600</v>
+      </c>
+      <c r="I23">
+        <v>0.5</v>
+      </c>
+      <c r="J23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B24">
         <v>301</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+      <c r="G24">
+        <v>3500</v>
+      </c>
+      <c r="H24">
+        <v>600</v>
+      </c>
+      <c r="I24">
+        <v>0.5</v>
+      </c>
+      <c r="J24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B25">
         <v>301</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>3500</v>
+      </c>
+      <c r="H25">
+        <v>600</v>
+      </c>
+      <c r="I25">
+        <v>0.5</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B26">
         <v>301</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26">
+        <v>10</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <v>3500</v>
+      </c>
+      <c r="H26">
+        <v>600</v>
+      </c>
+      <c r="I26">
+        <v>0.8</v>
+      </c>
+      <c r="J26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B27">
         <v>301</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27">
+        <v>3500</v>
+      </c>
+      <c r="H27">
+        <v>600</v>
+      </c>
+      <c r="I27">
+        <v>0.8</v>
+      </c>
+      <c r="J27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B28">
         <v>301</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+      <c r="G28">
+        <v>3500</v>
+      </c>
+      <c r="H28">
+        <v>600</v>
+      </c>
+      <c r="I28">
+        <v>0.8</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B29">
         <v>301</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>3500</v>
+      </c>
+      <c r="H29">
+        <v>600</v>
+      </c>
+      <c r="I29">
+        <v>0.2</v>
+      </c>
+      <c r="J29">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B30">
         <v>301</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>3500</v>
+      </c>
+      <c r="H30">
+        <v>600</v>
+      </c>
+      <c r="I30">
+        <v>0.2</v>
+      </c>
+      <c r="J30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B31">
         <v>301</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+      <c r="G31">
+        <v>3500</v>
+      </c>
+      <c r="H31">
+        <v>600</v>
+      </c>
+      <c r="I31">
+        <v>0.2</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B32">
         <v>301</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>10</v>
+      </c>
+      <c r="G32">
+        <v>3500</v>
+      </c>
+      <c r="H32">
+        <v>600</v>
+      </c>
+      <c r="I32">
+        <v>0.5</v>
+      </c>
+      <c r="J32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B33">
         <v>301</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>3500</v>
+      </c>
+      <c r="H33">
+        <v>600</v>
+      </c>
+      <c r="I33">
+        <v>0.5</v>
+      </c>
+      <c r="J33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B34">
         <v>301</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <v>3500</v>
+      </c>
+      <c r="H34">
+        <v>600</v>
+      </c>
+      <c r="I34">
+        <v>0.5</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B35">
         <v>301</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>3500</v>
+      </c>
+      <c r="H35">
+        <v>600</v>
+      </c>
+      <c r="I35">
+        <v>0.8</v>
+      </c>
+      <c r="J35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B36">
         <v>301</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>3500</v>
+      </c>
+      <c r="H36">
+        <v>600</v>
+      </c>
+      <c r="I36">
+        <v>0.8</v>
+      </c>
+      <c r="J36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B37">
         <v>301</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <v>3500</v>
+      </c>
+      <c r="H37">
+        <v>600</v>
+      </c>
+      <c r="I37">
+        <v>0.8</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B38">
         <v>301</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>3500</v>
+      </c>
+      <c r="H38">
+        <v>600</v>
+      </c>
+      <c r="I38">
+        <v>0.2</v>
+      </c>
+      <c r="J38">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B39">
         <v>301</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>3500</v>
+      </c>
+      <c r="H39">
+        <v>600</v>
+      </c>
+      <c r="I39">
+        <v>0.2</v>
+      </c>
+      <c r="J39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B40">
         <v>301</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E40">
+        <v>10</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>3500</v>
+      </c>
+      <c r="H40">
+        <v>600</v>
+      </c>
+      <c r="I40">
+        <v>0.2</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B41">
         <v>301</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>3500</v>
+      </c>
+      <c r="H41">
+        <v>600</v>
+      </c>
+      <c r="I41">
+        <v>0.5</v>
+      </c>
+      <c r="J41">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B42">
         <v>301</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42">
+        <v>10</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="G42">
+        <v>3500</v>
+      </c>
+      <c r="H42">
+        <v>600</v>
+      </c>
+      <c r="I42">
+        <v>0.5</v>
+      </c>
+      <c r="J42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B43">
         <v>301</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>3500</v>
+      </c>
+      <c r="H43">
+        <v>600</v>
+      </c>
+      <c r="I43">
+        <v>0.5</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B44">
         <v>301</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+      <c r="F44">
+        <v>10</v>
+      </c>
+      <c r="G44">
+        <v>3500</v>
+      </c>
+      <c r="H44">
+        <v>600</v>
+      </c>
+      <c r="I44">
+        <v>0.8</v>
+      </c>
+      <c r="J44">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B45">
         <v>301</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E45">
+        <v>10</v>
+      </c>
+      <c r="F45">
+        <v>10</v>
+      </c>
+      <c r="G45">
+        <v>3500</v>
+      </c>
+      <c r="H45">
+        <v>600</v>
+      </c>
+      <c r="I45">
+        <v>0.8</v>
+      </c>
+      <c r="J45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B46">
         <v>301</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+      <c r="G46">
+        <v>3500</v>
+      </c>
+      <c r="H46">
+        <v>600</v>
+      </c>
+      <c r="I46">
+        <v>0.8</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B47">
         <v>301</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47">
+        <v>10</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47">
+        <v>3500</v>
+      </c>
+      <c r="H47">
+        <v>600</v>
+      </c>
+      <c r="I47">
+        <v>0.2</v>
+      </c>
+      <c r="J47">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B48">
         <v>301</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48">
+        <v>10</v>
+      </c>
+      <c r="F48">
+        <v>10</v>
+      </c>
+      <c r="G48">
+        <v>3500</v>
+      </c>
+      <c r="H48">
+        <v>600</v>
+      </c>
+      <c r="I48">
+        <v>0.2</v>
+      </c>
+      <c r="J48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B49">
         <v>301</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>91</v>
+      </c>
+      <c r="D49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49">
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <v>10</v>
+      </c>
+      <c r="G49">
+        <v>3500</v>
+      </c>
+      <c r="H49">
+        <v>600</v>
+      </c>
+      <c r="I49">
+        <v>0.2</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B50">
         <v>301</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50">
+        <v>10</v>
+      </c>
+      <c r="F50">
+        <v>10</v>
+      </c>
+      <c r="G50">
+        <v>3500</v>
+      </c>
+      <c r="H50">
+        <v>600</v>
+      </c>
+      <c r="I50">
+        <v>0.5</v>
+      </c>
+      <c r="J50">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B51">
         <v>301</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51">
+        <v>10</v>
+      </c>
+      <c r="F51">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>3500</v>
+      </c>
+      <c r="H51">
+        <v>600</v>
+      </c>
+      <c r="I51">
+        <v>0.5</v>
+      </c>
+      <c r="J51">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B52">
         <v>301</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52">
+        <v>10</v>
+      </c>
+      <c r="F52">
+        <v>10</v>
+      </c>
+      <c r="G52">
+        <v>3500</v>
+      </c>
+      <c r="H52">
+        <v>600</v>
+      </c>
+      <c r="I52">
+        <v>0.5</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B53">
         <v>301</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53">
+        <v>10</v>
+      </c>
+      <c r="F53">
+        <v>10</v>
+      </c>
+      <c r="G53">
+        <v>3500</v>
+      </c>
+      <c r="H53">
+        <v>600</v>
+      </c>
+      <c r="I53">
+        <v>0.8</v>
+      </c>
+      <c r="J53">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B54">
         <v>301</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54">
+        <v>10</v>
+      </c>
+      <c r="F54">
+        <v>10</v>
+      </c>
+      <c r="G54">
+        <v>3500</v>
+      </c>
+      <c r="H54">
+        <v>600</v>
+      </c>
+      <c r="I54">
+        <v>0.8</v>
+      </c>
+      <c r="J54">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B55">
         <v>301</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+      <c r="D55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55">
+        <v>10</v>
+      </c>
+      <c r="F55">
+        <v>10</v>
+      </c>
+      <c r="G55">
+        <v>3500</v>
+      </c>
+      <c r="H55">
+        <v>600</v>
+      </c>
+      <c r="I55">
+        <v>0.8</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B56">
         <v>301</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56">
+        <v>10</v>
+      </c>
+      <c r="F56">
+        <v>10</v>
+      </c>
+      <c r="G56">
+        <v>3500</v>
+      </c>
+      <c r="H56">
+        <v>600</v>
+      </c>
+      <c r="I56">
+        <v>0.2</v>
+      </c>
+      <c r="J56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B57">
         <v>301</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" t="s">
+        <v>90</v>
+      </c>
+      <c r="E57">
+        <v>10</v>
+      </c>
+      <c r="F57">
+        <v>10</v>
+      </c>
+      <c r="G57">
+        <v>3500</v>
+      </c>
+      <c r="H57">
+        <v>600</v>
+      </c>
+      <c r="I57">
+        <v>0.2</v>
+      </c>
+      <c r="J57">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B58">
         <v>301</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" t="s">
+        <v>90</v>
+      </c>
+      <c r="E58">
+        <v>10</v>
+      </c>
+      <c r="F58">
+        <v>10</v>
+      </c>
+      <c r="G58">
+        <v>3500</v>
+      </c>
+      <c r="H58">
+        <v>600</v>
+      </c>
+      <c r="I58">
+        <v>0.2</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B59">
         <v>301</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" t="s">
+        <v>90</v>
+      </c>
+      <c r="E59">
+        <v>10</v>
+      </c>
+      <c r="F59">
+        <v>10</v>
+      </c>
+      <c r="G59">
+        <v>3500</v>
+      </c>
+      <c r="H59">
+        <v>600</v>
+      </c>
+      <c r="I59">
+        <v>0.5</v>
+      </c>
+      <c r="J59">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B60">
         <v>301</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" t="s">
+        <v>90</v>
+      </c>
+      <c r="E60">
+        <v>10</v>
+      </c>
+      <c r="F60">
+        <v>10</v>
+      </c>
+      <c r="G60">
+        <v>3500</v>
+      </c>
+      <c r="H60">
+        <v>600</v>
+      </c>
+      <c r="I60">
+        <v>0.5</v>
+      </c>
+      <c r="J60">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B61">
         <v>301</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61">
+        <v>10</v>
+      </c>
+      <c r="F61">
+        <v>10</v>
+      </c>
+      <c r="G61">
+        <v>3500</v>
+      </c>
+      <c r="H61">
+        <v>600</v>
+      </c>
+      <c r="I61">
+        <v>0.5</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B62">
         <v>301</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62">
+        <v>10</v>
+      </c>
+      <c r="F62">
+        <v>10</v>
+      </c>
+      <c r="G62">
+        <v>3500</v>
+      </c>
+      <c r="H62">
+        <v>600</v>
+      </c>
+      <c r="I62">
+        <v>0.8</v>
+      </c>
+      <c r="J62">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B63">
         <v>301</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63">
+        <v>10</v>
+      </c>
+      <c r="F63">
+        <v>10</v>
+      </c>
+      <c r="G63">
+        <v>3500</v>
+      </c>
+      <c r="H63">
+        <v>600</v>
+      </c>
+      <c r="I63">
+        <v>0.8</v>
+      </c>
+      <c r="J63">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B64">
         <v>301</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" t="s">
+        <v>90</v>
+      </c>
+      <c r="E64">
+        <v>10</v>
+      </c>
+      <c r="F64">
+        <v>10</v>
+      </c>
+      <c r="G64">
+        <v>3500</v>
+      </c>
+      <c r="H64">
+        <v>600</v>
+      </c>
+      <c r="I64">
+        <v>0.8</v>
+      </c>
+      <c r="J64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B65">
         <v>301</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65">
+        <v>10</v>
+      </c>
+      <c r="F65">
+        <v>10</v>
+      </c>
+      <c r="G65">
+        <v>3500</v>
+      </c>
+      <c r="H65">
+        <v>600</v>
+      </c>
+      <c r="I65">
+        <v>0.2</v>
+      </c>
+      <c r="J65">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B66">
         <v>301</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66">
+        <v>10</v>
+      </c>
+      <c r="F66">
+        <v>10</v>
+      </c>
+      <c r="G66">
+        <v>3500</v>
+      </c>
+      <c r="H66">
+        <v>600</v>
+      </c>
+      <c r="I66">
+        <v>0.2</v>
+      </c>
+      <c r="J66">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B67">
         <v>301</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67">
+        <v>10</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+      <c r="G67">
+        <v>3500</v>
+      </c>
+      <c r="H67">
+        <v>600</v>
+      </c>
+      <c r="I67">
+        <v>0.2</v>
+      </c>
+      <c r="J67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B68">
         <v>301</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68">
+        <v>10</v>
+      </c>
+      <c r="F68">
+        <v>10</v>
+      </c>
+      <c r="G68">
+        <v>3500</v>
+      </c>
+      <c r="H68">
+        <v>600</v>
+      </c>
+      <c r="I68">
+        <v>0.5</v>
+      </c>
+      <c r="J68">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B69">
         <v>301</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" t="s">
+        <v>91</v>
+      </c>
+      <c r="E69">
+        <v>10</v>
+      </c>
+      <c r="F69">
+        <v>10</v>
+      </c>
+      <c r="G69">
+        <v>3500</v>
+      </c>
+      <c r="H69">
+        <v>600</v>
+      </c>
+      <c r="I69">
+        <v>0.5</v>
+      </c>
+      <c r="J69">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B70">
         <v>301</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>92</v>
+      </c>
+      <c r="D70" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70">
+        <v>10</v>
+      </c>
+      <c r="F70">
+        <v>10</v>
+      </c>
+      <c r="G70">
+        <v>3500</v>
+      </c>
+      <c r="H70">
+        <v>600</v>
+      </c>
+      <c r="I70">
+        <v>0.5</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B71">
         <v>301</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D71" t="s">
+        <v>91</v>
+      </c>
+      <c r="E71">
+        <v>10</v>
+      </c>
+      <c r="F71">
+        <v>10</v>
+      </c>
+      <c r="G71">
+        <v>3500</v>
+      </c>
+      <c r="H71">
+        <v>600</v>
+      </c>
+      <c r="I71">
+        <v>0.8</v>
+      </c>
+      <c r="J71">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B72">
         <v>301</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72">
+        <v>10</v>
+      </c>
+      <c r="F72">
+        <v>10</v>
+      </c>
+      <c r="G72">
+        <v>3500</v>
+      </c>
+      <c r="H72">
+        <v>600</v>
+      </c>
+      <c r="I72">
+        <v>0.8</v>
+      </c>
+      <c r="J72">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B73">
         <v>301</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>92</v>
+      </c>
+      <c r="D73" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73">
+        <v>10</v>
+      </c>
+      <c r="F73">
+        <v>10</v>
+      </c>
+      <c r="G73">
+        <v>3500</v>
+      </c>
+      <c r="H73">
+        <v>600</v>
+      </c>
+      <c r="I73">
+        <v>0.8</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B74">
         <v>301</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74">
+        <v>10</v>
+      </c>
+      <c r="F74">
+        <v>10</v>
+      </c>
+      <c r="G74">
+        <v>3500</v>
+      </c>
+      <c r="H74">
+        <v>600</v>
+      </c>
+      <c r="I74">
+        <v>0.2</v>
+      </c>
+      <c r="J74">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B75">
         <v>301</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" t="s">
+        <v>92</v>
+      </c>
+      <c r="E75">
+        <v>10</v>
+      </c>
+      <c r="F75">
+        <v>10</v>
+      </c>
+      <c r="G75">
+        <v>3500</v>
+      </c>
+      <c r="H75">
+        <v>600</v>
+      </c>
+      <c r="I75">
+        <v>0.2</v>
+      </c>
+      <c r="J75">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B76">
         <v>301</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>92</v>
+      </c>
+      <c r="D76" t="s">
+        <v>92</v>
+      </c>
+      <c r="E76">
+        <v>10</v>
+      </c>
+      <c r="F76">
+        <v>10</v>
+      </c>
+      <c r="G76">
+        <v>3500</v>
+      </c>
+      <c r="H76">
+        <v>600</v>
+      </c>
+      <c r="I76">
+        <v>0.2</v>
+      </c>
+      <c r="J76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B77">
         <v>301</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>92</v>
+      </c>
+      <c r="D77" t="s">
+        <v>92</v>
+      </c>
+      <c r="E77">
+        <v>10</v>
+      </c>
+      <c r="F77">
+        <v>10</v>
+      </c>
+      <c r="G77">
+        <v>3500</v>
+      </c>
+      <c r="H77">
+        <v>600</v>
+      </c>
+      <c r="I77">
+        <v>0.5</v>
+      </c>
+      <c r="J77">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B78">
         <v>301</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" t="s">
+        <v>92</v>
+      </c>
+      <c r="E78">
+        <v>10</v>
+      </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
+      <c r="G78">
+        <v>3500</v>
+      </c>
+      <c r="H78">
+        <v>600</v>
+      </c>
+      <c r="I78">
+        <v>0.5</v>
+      </c>
+      <c r="J78">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B79">
         <v>301</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>92</v>
+      </c>
+      <c r="D79" t="s">
+        <v>92</v>
+      </c>
+      <c r="E79">
+        <v>10</v>
+      </c>
+      <c r="F79">
+        <v>10</v>
+      </c>
+      <c r="G79">
+        <v>3500</v>
+      </c>
+      <c r="H79">
+        <v>600</v>
+      </c>
+      <c r="I79">
+        <v>0.5</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B80">
         <v>301</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>92</v>
+      </c>
+      <c r="D80" t="s">
+        <v>92</v>
+      </c>
+      <c r="E80">
+        <v>10</v>
+      </c>
+      <c r="F80">
+        <v>10</v>
+      </c>
+      <c r="G80">
+        <v>3500</v>
+      </c>
+      <c r="H80">
+        <v>600</v>
+      </c>
+      <c r="I80">
+        <v>0.8</v>
+      </c>
+      <c r="J80">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B81">
         <v>301</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>92</v>
+      </c>
+      <c r="D81" t="s">
+        <v>92</v>
+      </c>
+      <c r="E81">
+        <v>10</v>
+      </c>
+      <c r="F81">
+        <v>10</v>
+      </c>
+      <c r="G81">
+        <v>3500</v>
+      </c>
+      <c r="H81">
+        <v>600</v>
+      </c>
+      <c r="I81">
+        <v>0.8</v>
+      </c>
+      <c r="J81">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B82">
         <v>301</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B83">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B84">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B85">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B86">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B87">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B88">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B89">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B90">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B91">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B93">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B94">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B95">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B96">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B97">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B98">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B99">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B100">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B101">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B102">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B103">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B104">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B105">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B106">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B107">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B108">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B109">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
+      <c r="C82" t="s">
+        <v>92</v>
+      </c>
+      <c r="D82" t="s">
+        <v>92</v>
+      </c>
+      <c r="E82">
+        <v>10</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <v>3500</v>
+      </c>
+      <c r="H82">
+        <v>600</v>
+      </c>
+      <c r="I82">
+        <v>0.8</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor adjustments to balance out the advantages of each animal type
</commit_message>
<xml_diff>
--- a/InitialTestValues.xlsx
+++ b/InitialTestValues.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\Predator_Prey_ExpSARSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridan\Desktop\TESTDISOO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6ADC06-717D-415E-9CDF-07BB049AE90E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1570286-4410-4026-8DC8-BEDB9A839D73}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10395" xr2:uid="{2755E7A2-B65B-4843-98C1-1521C9C3621F}"/>
   </bookViews>
@@ -668,7 +668,7 @@
   <dimension ref="A1:M83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +678,8 @@
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -744,7 +745,7 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>30</v>
@@ -753,7 +754,7 @@
         <v>50</v>
       </c>
       <c r="J2">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K2">
         <v>600</v>
@@ -785,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <v>30</v>
@@ -794,7 +795,7 @@
         <v>50</v>
       </c>
       <c r="J3">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K3">
         <v>600</v>
@@ -826,7 +827,7 @@
         <v>10</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H4">
         <v>30</v>
@@ -835,7 +836,7 @@
         <v>50</v>
       </c>
       <c r="J4">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K4">
         <v>600</v>
@@ -867,7 +868,7 @@
         <v>10</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>30</v>
@@ -876,7 +877,7 @@
         <v>50</v>
       </c>
       <c r="J5">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K5">
         <v>600</v>
@@ -908,7 +909,7 @@
         <v>10</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H6">
         <v>30</v>
@@ -917,7 +918,7 @@
         <v>50</v>
       </c>
       <c r="J6">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K6">
         <v>600</v>
@@ -949,7 +950,7 @@
         <v>10</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <v>30</v>
@@ -958,7 +959,7 @@
         <v>50</v>
       </c>
       <c r="J7">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K7">
         <v>600</v>
@@ -990,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <v>30</v>
@@ -999,7 +1000,7 @@
         <v>50</v>
       </c>
       <c r="J8">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K8">
         <v>600</v>
@@ -1031,7 +1032,7 @@
         <v>10</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H9">
         <v>30</v>
@@ -1040,7 +1041,7 @@
         <v>50</v>
       </c>
       <c r="J9">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K9">
         <v>600</v>
@@ -1072,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <v>30</v>
@@ -1081,7 +1082,7 @@
         <v>50</v>
       </c>
       <c r="J10">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K10">
         <v>600</v>
@@ -1113,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>30</v>
@@ -1122,7 +1123,7 @@
         <v>50</v>
       </c>
       <c r="J11">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K11">
         <v>600</v>
@@ -1154,7 +1155,7 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H12">
         <v>30</v>
@@ -1163,7 +1164,7 @@
         <v>50</v>
       </c>
       <c r="J12">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K12">
         <v>600</v>
@@ -1195,7 +1196,7 @@
         <v>10</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H13">
         <v>30</v>
@@ -1204,7 +1205,7 @@
         <v>50</v>
       </c>
       <c r="J13">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K13">
         <v>600</v>
@@ -1236,7 +1237,7 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H14">
         <v>30</v>
@@ -1245,7 +1246,7 @@
         <v>50</v>
       </c>
       <c r="J14">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K14">
         <v>600</v>
@@ -1277,7 +1278,7 @@
         <v>10</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H15">
         <v>30</v>
@@ -1286,7 +1287,7 @@
         <v>50</v>
       </c>
       <c r="J15">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K15">
         <v>600</v>
@@ -1318,7 +1319,7 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H16">
         <v>30</v>
@@ -1327,7 +1328,7 @@
         <v>50</v>
       </c>
       <c r="J16">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K16">
         <v>600</v>
@@ -1359,7 +1360,7 @@
         <v>10</v>
       </c>
       <c r="G17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H17">
         <v>30</v>
@@ -1368,7 +1369,7 @@
         <v>50</v>
       </c>
       <c r="J17">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K17">
         <v>600</v>
@@ -1400,7 +1401,7 @@
         <v>10</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H18">
         <v>30</v>
@@ -1409,7 +1410,7 @@
         <v>50</v>
       </c>
       <c r="J18">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K18">
         <v>600</v>
@@ -1441,7 +1442,7 @@
         <v>10</v>
       </c>
       <c r="G19">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H19">
         <v>30</v>
@@ -1450,7 +1451,7 @@
         <v>50</v>
       </c>
       <c r="J19">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K19">
         <v>600</v>
@@ -1482,7 +1483,7 @@
         <v>10</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H20">
         <v>30</v>
@@ -1491,7 +1492,7 @@
         <v>50</v>
       </c>
       <c r="J20">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K20">
         <v>600</v>
@@ -1523,7 +1524,7 @@
         <v>10</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H21">
         <v>30</v>
@@ -1532,7 +1533,7 @@
         <v>50</v>
       </c>
       <c r="J21">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K21">
         <v>600</v>
@@ -1564,7 +1565,7 @@
         <v>10</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H22">
         <v>30</v>
@@ -1573,7 +1574,7 @@
         <v>50</v>
       </c>
       <c r="J22">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K22">
         <v>600</v>
@@ -1605,7 +1606,7 @@
         <v>10</v>
       </c>
       <c r="G23">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H23">
         <v>30</v>
@@ -1614,7 +1615,7 @@
         <v>50</v>
       </c>
       <c r="J23">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K23">
         <v>600</v>
@@ -1646,7 +1647,7 @@
         <v>10</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H24">
         <v>30</v>
@@ -1655,7 +1656,7 @@
         <v>50</v>
       </c>
       <c r="J24">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K24">
         <v>600</v>
@@ -1687,7 +1688,7 @@
         <v>10</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H25">
         <v>30</v>
@@ -1696,7 +1697,7 @@
         <v>50</v>
       </c>
       <c r="J25">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K25">
         <v>600</v>
@@ -1728,7 +1729,7 @@
         <v>10</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H26">
         <v>30</v>
@@ -1737,7 +1738,7 @@
         <v>50</v>
       </c>
       <c r="J26">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K26">
         <v>600</v>
@@ -1769,7 +1770,7 @@
         <v>10</v>
       </c>
       <c r="G27">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H27">
         <v>30</v>
@@ -1778,7 +1779,7 @@
         <v>50</v>
       </c>
       <c r="J27">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K27">
         <v>600</v>
@@ -1810,7 +1811,7 @@
         <v>10</v>
       </c>
       <c r="G28">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H28">
         <v>30</v>
@@ -1819,7 +1820,7 @@
         <v>50</v>
       </c>
       <c r="J28">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K28">
         <v>600</v>
@@ -1851,7 +1852,7 @@
         <v>10</v>
       </c>
       <c r="G29">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H29">
         <v>30</v>
@@ -1860,7 +1861,7 @@
         <v>50</v>
       </c>
       <c r="J29">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K29">
         <v>600</v>
@@ -1892,7 +1893,7 @@
         <v>10</v>
       </c>
       <c r="G30">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H30">
         <v>30</v>
@@ -1901,7 +1902,7 @@
         <v>50</v>
       </c>
       <c r="J30">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K30">
         <v>600</v>
@@ -1933,7 +1934,7 @@
         <v>10</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H31">
         <v>30</v>
@@ -1942,7 +1943,7 @@
         <v>50</v>
       </c>
       <c r="J31">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K31">
         <v>600</v>
@@ -1974,7 +1975,7 @@
         <v>10</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H32">
         <v>30</v>
@@ -1983,7 +1984,7 @@
         <v>50</v>
       </c>
       <c r="J32">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K32">
         <v>600</v>
@@ -2015,7 +2016,7 @@
         <v>10</v>
       </c>
       <c r="G33">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H33">
         <v>30</v>
@@ -2024,7 +2025,7 @@
         <v>50</v>
       </c>
       <c r="J33">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K33">
         <v>600</v>
@@ -2056,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="G34">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H34">
         <v>30</v>
@@ -2065,7 +2066,7 @@
         <v>50</v>
       </c>
       <c r="J34">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K34">
         <v>600</v>
@@ -2097,7 +2098,7 @@
         <v>10</v>
       </c>
       <c r="G35">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H35">
         <v>30</v>
@@ -2106,7 +2107,7 @@
         <v>50</v>
       </c>
       <c r="J35">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K35">
         <v>600</v>
@@ -2138,7 +2139,7 @@
         <v>10</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H36">
         <v>30</v>
@@ -2147,7 +2148,7 @@
         <v>50</v>
       </c>
       <c r="J36">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K36">
         <v>600</v>
@@ -2179,7 +2180,7 @@
         <v>10</v>
       </c>
       <c r="G37">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H37">
         <v>30</v>
@@ -2188,7 +2189,7 @@
         <v>50</v>
       </c>
       <c r="J37">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K37">
         <v>600</v>
@@ -2220,7 +2221,7 @@
         <v>10</v>
       </c>
       <c r="G38">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H38">
         <v>30</v>
@@ -2229,7 +2230,7 @@
         <v>50</v>
       </c>
       <c r="J38">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K38">
         <v>600</v>
@@ -2261,7 +2262,7 @@
         <v>10</v>
       </c>
       <c r="G39">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H39">
         <v>30</v>
@@ -2270,7 +2271,7 @@
         <v>50</v>
       </c>
       <c r="J39">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K39">
         <v>600</v>
@@ -2302,7 +2303,7 @@
         <v>10</v>
       </c>
       <c r="G40">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H40">
         <v>30</v>
@@ -2311,7 +2312,7 @@
         <v>50</v>
       </c>
       <c r="J40">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K40">
         <v>600</v>
@@ -2343,7 +2344,7 @@
         <v>10</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H41">
         <v>30</v>
@@ -2352,7 +2353,7 @@
         <v>50</v>
       </c>
       <c r="J41">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K41">
         <v>600</v>
@@ -2384,7 +2385,7 @@
         <v>10</v>
       </c>
       <c r="G42">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H42">
         <v>30</v>
@@ -2393,7 +2394,7 @@
         <v>50</v>
       </c>
       <c r="J42">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K42">
         <v>600</v>
@@ -2425,7 +2426,7 @@
         <v>10</v>
       </c>
       <c r="G43">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H43">
         <v>30</v>
@@ -2434,7 +2435,7 @@
         <v>50</v>
       </c>
       <c r="J43">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K43">
         <v>600</v>
@@ -2466,7 +2467,7 @@
         <v>10</v>
       </c>
       <c r="G44">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H44">
         <v>30</v>
@@ -2475,7 +2476,7 @@
         <v>50</v>
       </c>
       <c r="J44">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K44">
         <v>600</v>
@@ -2507,7 +2508,7 @@
         <v>10</v>
       </c>
       <c r="G45">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H45">
         <v>30</v>
@@ -2516,7 +2517,7 @@
         <v>50</v>
       </c>
       <c r="J45">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K45">
         <v>600</v>
@@ -2548,7 +2549,7 @@
         <v>10</v>
       </c>
       <c r="G46">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H46">
         <v>30</v>
@@ -2557,7 +2558,7 @@
         <v>50</v>
       </c>
       <c r="J46">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K46">
         <v>600</v>
@@ -2589,7 +2590,7 @@
         <v>10</v>
       </c>
       <c r="G47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H47">
         <v>30</v>
@@ -2598,7 +2599,7 @@
         <v>50</v>
       </c>
       <c r="J47">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K47">
         <v>600</v>
@@ -2630,7 +2631,7 @@
         <v>10</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H48">
         <v>30</v>
@@ -2639,7 +2640,7 @@
         <v>50</v>
       </c>
       <c r="J48">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K48">
         <v>600</v>
@@ -2671,7 +2672,7 @@
         <v>10</v>
       </c>
       <c r="G49">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H49">
         <v>30</v>
@@ -2680,7 +2681,7 @@
         <v>50</v>
       </c>
       <c r="J49">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K49">
         <v>600</v>
@@ -2712,7 +2713,7 @@
         <v>10</v>
       </c>
       <c r="G50">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H50">
         <v>30</v>
@@ -2721,7 +2722,7 @@
         <v>50</v>
       </c>
       <c r="J50">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K50">
         <v>600</v>
@@ -2753,7 +2754,7 @@
         <v>10</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H51">
         <v>30</v>
@@ -2762,7 +2763,7 @@
         <v>50</v>
       </c>
       <c r="J51">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K51">
         <v>600</v>
@@ -2794,7 +2795,7 @@
         <v>10</v>
       </c>
       <c r="G52">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H52">
         <v>30</v>
@@ -2803,7 +2804,7 @@
         <v>50</v>
       </c>
       <c r="J52">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K52">
         <v>600</v>
@@ -2835,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="G53">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H53">
         <v>30</v>
@@ -2844,7 +2845,7 @@
         <v>50</v>
       </c>
       <c r="J53">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K53">
         <v>600</v>
@@ -2876,7 +2877,7 @@
         <v>10</v>
       </c>
       <c r="G54">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H54">
         <v>30</v>
@@ -2885,7 +2886,7 @@
         <v>50</v>
       </c>
       <c r="J54">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K54">
         <v>600</v>
@@ -2917,7 +2918,7 @@
         <v>10</v>
       </c>
       <c r="G55">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H55">
         <v>30</v>
@@ -2926,7 +2927,7 @@
         <v>50</v>
       </c>
       <c r="J55">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K55">
         <v>600</v>
@@ -2958,7 +2959,7 @@
         <v>10</v>
       </c>
       <c r="G56">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H56">
         <v>30</v>
@@ -2967,7 +2968,7 @@
         <v>50</v>
       </c>
       <c r="J56">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K56">
         <v>600</v>
@@ -2999,7 +3000,7 @@
         <v>10</v>
       </c>
       <c r="G57">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H57">
         <v>30</v>
@@ -3008,7 +3009,7 @@
         <v>50</v>
       </c>
       <c r="J57">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K57">
         <v>600</v>
@@ -3040,7 +3041,7 @@
         <v>10</v>
       </c>
       <c r="G58">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H58">
         <v>30</v>
@@ -3049,7 +3050,7 @@
         <v>50</v>
       </c>
       <c r="J58">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K58">
         <v>600</v>
@@ -3081,7 +3082,7 @@
         <v>10</v>
       </c>
       <c r="G59">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H59">
         <v>30</v>
@@ -3090,7 +3091,7 @@
         <v>50</v>
       </c>
       <c r="J59">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K59">
         <v>600</v>
@@ -3122,7 +3123,7 @@
         <v>10</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H60">
         <v>30</v>
@@ -3131,7 +3132,7 @@
         <v>50</v>
       </c>
       <c r="J60">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K60">
         <v>600</v>
@@ -3163,7 +3164,7 @@
         <v>10</v>
       </c>
       <c r="G61">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H61">
         <v>30</v>
@@ -3172,7 +3173,7 @@
         <v>50</v>
       </c>
       <c r="J61">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K61">
         <v>600</v>
@@ -3204,7 +3205,7 @@
         <v>10</v>
       </c>
       <c r="G62">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H62">
         <v>30</v>
@@ -3213,7 +3214,7 @@
         <v>50</v>
       </c>
       <c r="J62">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K62">
         <v>600</v>
@@ -3245,7 +3246,7 @@
         <v>10</v>
       </c>
       <c r="G63">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H63">
         <v>30</v>
@@ -3254,7 +3255,7 @@
         <v>50</v>
       </c>
       <c r="J63">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K63">
         <v>600</v>
@@ -3286,7 +3287,7 @@
         <v>10</v>
       </c>
       <c r="G64">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H64">
         <v>30</v>
@@ -3295,7 +3296,7 @@
         <v>50</v>
       </c>
       <c r="J64">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K64">
         <v>600</v>
@@ -3327,7 +3328,7 @@
         <v>10</v>
       </c>
       <c r="G65">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H65">
         <v>30</v>
@@ -3336,7 +3337,7 @@
         <v>50</v>
       </c>
       <c r="J65">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K65">
         <v>600</v>
@@ -3368,7 +3369,7 @@
         <v>10</v>
       </c>
       <c r="G66">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H66">
         <v>30</v>
@@ -3377,7 +3378,7 @@
         <v>50</v>
       </c>
       <c r="J66">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K66">
         <v>600</v>
@@ -3409,7 +3410,7 @@
         <v>10</v>
       </c>
       <c r="G67">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H67">
         <v>30</v>
@@ -3418,7 +3419,7 @@
         <v>50</v>
       </c>
       <c r="J67">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K67">
         <v>600</v>
@@ -3450,7 +3451,7 @@
         <v>10</v>
       </c>
       <c r="G68">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H68">
         <v>30</v>
@@ -3459,7 +3460,7 @@
         <v>50</v>
       </c>
       <c r="J68">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K68">
         <v>600</v>
@@ -3491,7 +3492,7 @@
         <v>10</v>
       </c>
       <c r="G69">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H69">
         <v>30</v>
@@ -3500,7 +3501,7 @@
         <v>50</v>
       </c>
       <c r="J69">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K69">
         <v>600</v>
@@ -3532,7 +3533,7 @@
         <v>10</v>
       </c>
       <c r="G70">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H70">
         <v>30</v>
@@ -3541,7 +3542,7 @@
         <v>50</v>
       </c>
       <c r="J70">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K70">
         <v>600</v>
@@ -3573,7 +3574,7 @@
         <v>10</v>
       </c>
       <c r="G71">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H71">
         <v>30</v>
@@ -3582,7 +3583,7 @@
         <v>50</v>
       </c>
       <c r="J71">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K71">
         <v>600</v>
@@ -3614,7 +3615,7 @@
         <v>10</v>
       </c>
       <c r="G72">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H72">
         <v>30</v>
@@ -3623,7 +3624,7 @@
         <v>50</v>
       </c>
       <c r="J72">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K72">
         <v>600</v>
@@ -3655,7 +3656,7 @@
         <v>10</v>
       </c>
       <c r="G73">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H73">
         <v>30</v>
@@ -3664,7 +3665,7 @@
         <v>50</v>
       </c>
       <c r="J73">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K73">
         <v>600</v>
@@ -3696,7 +3697,7 @@
         <v>10</v>
       </c>
       <c r="G74">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H74">
         <v>30</v>
@@ -3705,7 +3706,7 @@
         <v>50</v>
       </c>
       <c r="J74">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K74">
         <v>600</v>
@@ -3737,7 +3738,7 @@
         <v>10</v>
       </c>
       <c r="G75">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H75">
         <v>30</v>
@@ -3746,7 +3747,7 @@
         <v>50</v>
       </c>
       <c r="J75">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K75">
         <v>600</v>
@@ -3778,7 +3779,7 @@
         <v>10</v>
       </c>
       <c r="G76">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H76">
         <v>30</v>
@@ -3787,7 +3788,7 @@
         <v>50</v>
       </c>
       <c r="J76">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K76">
         <v>600</v>
@@ -3819,7 +3820,7 @@
         <v>10</v>
       </c>
       <c r="G77">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H77">
         <v>30</v>
@@ -3828,7 +3829,7 @@
         <v>50</v>
       </c>
       <c r="J77">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K77">
         <v>600</v>
@@ -3860,7 +3861,7 @@
         <v>10</v>
       </c>
       <c r="G78">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H78">
         <v>30</v>
@@ -3869,7 +3870,7 @@
         <v>50</v>
       </c>
       <c r="J78">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K78">
         <v>600</v>
@@ -3901,7 +3902,7 @@
         <v>10</v>
       </c>
       <c r="G79">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H79">
         <v>30</v>
@@ -3910,7 +3911,7 @@
         <v>50</v>
       </c>
       <c r="J79">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K79">
         <v>600</v>
@@ -3942,7 +3943,7 @@
         <v>10</v>
       </c>
       <c r="G80">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H80">
         <v>30</v>
@@ -3951,7 +3952,7 @@
         <v>50</v>
       </c>
       <c r="J80">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K80">
         <v>600</v>
@@ -3983,7 +3984,7 @@
         <v>10</v>
       </c>
       <c r="G81">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H81">
         <v>30</v>
@@ -3992,7 +3993,7 @@
         <v>50</v>
       </c>
       <c r="J81">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K81">
         <v>600</v>
@@ -4024,7 +4025,7 @@
         <v>10</v>
       </c>
       <c r="G82">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H82">
         <v>30</v>
@@ -4033,7 +4034,7 @@
         <v>50</v>
       </c>
       <c r="J82">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="K82">
         <v>600</v>

</xml_diff>